<commit_message>
train new human model
</commit_message>
<xml_diff>
--- a/python_code/data/all_agents_score.xlsx
+++ b/python_code/data/all_agents_score.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:D137"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1695,14 +1695,14 @@
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
         <is>
-          <t>-N3ub2xMDKwS4Skdp6kB</t>
+          <t>-N3ubJNnx-yyc4GxXE8A</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C71" t="n">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
@@ -1713,32 +1713,32 @@
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
         <is>
-          <t>-N3ubJNnx-yyc4GxXE8A</t>
+          <t>-N3ubia-MvaGiUj1I_ST</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C72" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>closest</t>
+          <t>random</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
         <is>
-          <t>-N3ubhTqk34i3VI-9wIA</t>
+          <t>-N3ufEGQtV1mLdaLJvG0</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C73" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
@@ -1749,14 +1749,14 @@
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
         <is>
-          <t>-N3ubia-MvaGiUj1I_ST</t>
+          <t>-N3ufKTNK-9JZt9XRbVi</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C74" t="n">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
@@ -1767,68 +1767,68 @@
     <row r="75">
       <c r="A75" s="1" t="inlineStr">
         <is>
-          <t>-N3ufEGQtV1mLdaLJvG0</t>
+          <t>-N3ufR2J8fZXMIOEIv4B</t>
         </is>
       </c>
       <c r="B75" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C75" t="n">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>random</t>
+          <t>follow_stag</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="inlineStr">
         <is>
-          <t>-N3ufKTNK-9JZt9XRbVi</t>
+          <t>-N3ugOCIpM6xZeVfkGnp</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="C76" t="n">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>random</t>
+          <t>closest</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
         <is>
-          <t>-N3ufR2J8fZXMIOEIv4B</t>
+          <t>-N3uhXjnS89p_LGEUlOY</t>
         </is>
       </c>
       <c r="B77" t="n">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="C77" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>follow_stag</t>
+          <t>closest</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="inlineStr">
         <is>
-          <t>-N3ugOCIpM6xZeVfkGnp</t>
+          <t>-N3uhm198VZ44J_Vh6co</t>
         </is>
       </c>
       <c r="B78" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C78" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
@@ -1839,86 +1839,86 @@
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
         <is>
-          <t>-N3uhXjnS89p_LGEUlOY</t>
+          <t>-N3uhxvCsCnmNwN-PucK</t>
         </is>
       </c>
       <c r="B79" t="n">
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="C79" t="n">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>closest</t>
+          <t>follow_stag</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="inlineStr">
         <is>
-          <t>-N3uhm198VZ44J_Vh6co</t>
+          <t>-N3uigwoZyA9bvToWMaj</t>
         </is>
       </c>
       <c r="B80" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C80" t="n">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>closest</t>
+          <t>follow_stag</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="inlineStr">
         <is>
-          <t>-N3uhxvCsCnmNwN-PucK</t>
+          <t>-N3uk5j81irIpDQsd5rk</t>
         </is>
       </c>
       <c r="B81" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C81" t="n">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>follow_stag</t>
+          <t>random</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="inlineStr">
         <is>
-          <t>-N3uigwoZyA9bvToWMaj</t>
+          <t>-N3uk7zhB-eUTaVREa9U</t>
         </is>
       </c>
       <c r="B82" t="n">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="C82" t="n">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>follow_stag</t>
+          <t>random</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="inlineStr">
         <is>
-          <t>-N3uk5j81irIpDQsd5rk</t>
+          <t>-N3ukPfXhxNoaSabbk3V</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C83" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
@@ -1929,32 +1929,32 @@
     <row r="84">
       <c r="A84" s="1" t="inlineStr">
         <is>
-          <t>-N3uk7zhB-eUTaVREa9U</t>
+          <t>-N3ukfzQ3CN3SZhuJ2mR</t>
         </is>
       </c>
       <c r="B84" t="n">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C84" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>random</t>
+          <t>closest</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="inlineStr">
         <is>
-          <t>-N3ukPfXhxNoaSabbk3V</t>
+          <t>-N3ulJFf3urflvJxqB0q</t>
         </is>
       </c>
       <c r="B85" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C85" t="n">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
@@ -1965,14 +1965,14 @@
     <row r="86">
       <c r="A86" s="1" t="inlineStr">
         <is>
-          <t>-N3ukfzQ3CN3SZhuJ2mR</t>
+          <t>-N3um7LSvUBerrQ14v33</t>
         </is>
       </c>
       <c r="B86" t="n">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C86" t="n">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
@@ -1983,104 +1983,104 @@
     <row r="87">
       <c r="A87" s="1" t="inlineStr">
         <is>
-          <t>-N3ulJFf3urflvJxqB0q</t>
+          <t>-N3um7bjC3bKz83A5QmH</t>
         </is>
       </c>
       <c r="B87" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C87" t="n">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>random</t>
+          <t>follow_stag</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="inlineStr">
         <is>
-          <t>-N3um7LSvUBerrQ14v33</t>
+          <t>-N3umgI6PwHgE_vrnPx8</t>
         </is>
       </c>
       <c r="B88" t="n">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C88" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>closest</t>
+          <t>follow_stag</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="inlineStr">
         <is>
-          <t>-N3um7bjC3bKz83A5QmH</t>
+          <t>-N3umvTpwkm2rIlM7PG_</t>
         </is>
       </c>
       <c r="B89" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C89" t="n">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>follow_stag</t>
+          <t>closest</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="inlineStr">
         <is>
-          <t>-N3umgI6PwHgE_vrnPx8</t>
+          <t>-N3upYgfnpe6-O9VkNxr</t>
         </is>
       </c>
       <c r="B90" t="n">
+        <v>30</v>
+      </c>
+      <c r="C90" t="n">
         <v>29</v>
       </c>
-      <c r="C90" t="n">
-        <v>30</v>
-      </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>follow_stag</t>
+          <t>closest</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="inlineStr">
         <is>
-          <t>-N3umvTpwkm2rIlM7PG_</t>
+          <t>-N3upqD_fUASo7nNUCTV</t>
         </is>
       </c>
       <c r="B91" t="n">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C91" t="n">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>closest</t>
+          <t>follow_stag</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="inlineStr">
         <is>
-          <t>-N3upYgfnpe6-O9VkNxr</t>
+          <t>-N3usmEAOPlnHaohno-X</t>
         </is>
       </c>
       <c r="B92" t="n">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C92" t="n">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
@@ -2091,32 +2091,32 @@
     <row r="93">
       <c r="A93" s="1" t="inlineStr">
         <is>
-          <t>-N3upqD_fUASo7nNUCTV</t>
+          <t>-N3uuFquU_oj8cLxKm9S</t>
         </is>
       </c>
       <c r="B93" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C93" t="n">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>follow_stag</t>
+          <t>closest</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="inlineStr">
         <is>
-          <t>-N3usmEAOPlnHaohno-X</t>
+          <t>-N3v-ouUbrkNUDP6_W7P</t>
         </is>
       </c>
       <c r="B94" t="n">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="C94" t="n">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
@@ -2127,14 +2127,14 @@
     <row r="95">
       <c r="A95" s="1" t="inlineStr">
         <is>
-          <t>-N3uuFquU_oj8cLxKm9S</t>
+          <t>-N3v7NW69veDQNJNnpaO</t>
         </is>
       </c>
       <c r="B95" t="n">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C95" t="n">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
@@ -2145,50 +2145,50 @@
     <row r="96">
       <c r="A96" s="1" t="inlineStr">
         <is>
-          <t>-N3v-ouUbrkNUDP6_W7P</t>
+          <t>-N3vEf547tTerzaHQk0o</t>
         </is>
       </c>
       <c r="B96" t="n">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="C96" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>closest</t>
+          <t>random</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="inlineStr">
         <is>
-          <t>-N3v7NW69veDQNJNnpaO</t>
+          <t>-N3vP08kpF1JCjMg8zi0</t>
         </is>
       </c>
       <c r="B97" t="n">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C97" t="n">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>closest</t>
+          <t>follow_stag</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="inlineStr">
         <is>
-          <t>-N3vEf547tTerzaHQk0o</t>
+          <t>-N3vS2etXaI8llgn0qrz</t>
         </is>
       </c>
       <c r="B98" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C98" t="n">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D98" t="inlineStr">
         <is>
@@ -2199,54 +2199,702 @@
     <row r="99">
       <c r="A99" s="1" t="inlineStr">
         <is>
-          <t>-N3vP08kpF1JCjMg8zi0</t>
+          <t>-N3xR5UfHcnRH5BS3meJ</t>
         </is>
       </c>
       <c r="B99" t="n">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C99" t="n">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>follow_stag</t>
+          <t>closest</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="inlineStr">
         <is>
-          <t>-N3vS2etXaI8llgn0qrz</t>
+          <t>-N60-G76Th6s4ECC8STb</t>
         </is>
       </c>
       <c r="B100" t="n">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C100" t="n">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>random</t>
+          <t>closest</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="inlineStr">
         <is>
-          <t>-N3xR5UfHcnRH5BS3meJ</t>
+          <t>-N60-_gZ6U9nuizjY7bg</t>
         </is>
       </c>
       <c r="B101" t="n">
+        <v>7</v>
+      </c>
+      <c r="C101" t="n">
+        <v>22</v>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>random</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="inlineStr">
+        <is>
+          <t>-N60-i15gPVYo-1ZsNm8</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>31</v>
+      </c>
+      <c r="C102" t="n">
+        <v>27</v>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>closest</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="inlineStr">
+        <is>
+          <t>-N60-v_uOv2Z39ybuhSn</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
         <v>26</v>
       </c>
-      <c r="C101" t="n">
+      <c r="C103" t="n">
+        <v>35</v>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>follow_stag</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="inlineStr">
+        <is>
+          <t>-N600-7WYheXOKVgUg4K</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>18</v>
+      </c>
+      <c r="C104" t="n">
+        <v>29</v>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>closest</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="inlineStr">
+        <is>
+          <t>-N6003NVcwRQOstmQZia</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>26</v>
+      </c>
+      <c r="C105" t="n">
+        <v>20</v>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>closest</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="inlineStr">
+        <is>
+          <t>-N600GBERJ9DLzOIQDGI</t>
+        </is>
+      </c>
+      <c r="B106" t="n">
+        <v>29</v>
+      </c>
+      <c r="C106" t="n">
+        <v>18</v>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>closest</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="inlineStr">
+        <is>
+          <t>-N600QSf7tAXOMz9sN03</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>9</v>
+      </c>
+      <c r="C107" t="n">
+        <v>20</v>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>random</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="inlineStr">
+        <is>
+          <t>-N600VFUe-9i_EX2uZc1</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>22</v>
+      </c>
+      <c r="C108" t="n">
+        <v>17</v>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>closest</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="inlineStr">
+        <is>
+          <t>-N600akCmcpWvfUvyXSr</t>
+        </is>
+      </c>
+      <c r="B109" t="n">
+        <v>6</v>
+      </c>
+      <c r="C109" t="n">
+        <v>24</v>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>random</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="inlineStr">
+        <is>
+          <t>-N600eCV-aGYL8Z_aMNO</t>
+        </is>
+      </c>
+      <c r="B110" t="n">
+        <v>27</v>
+      </c>
+      <c r="C110" t="n">
+        <v>33</v>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>closest</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="inlineStr">
+        <is>
+          <t>-N600j_csYpnoOceKUEq</t>
+        </is>
+      </c>
+      <c r="B111" t="n">
+        <v>30</v>
+      </c>
+      <c r="C111" t="n">
+        <v>33</v>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>follow_stag</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="inlineStr">
+        <is>
+          <t>-N600kVz4mhm0haN1UoC</t>
+        </is>
+      </c>
+      <c r="B112" t="n">
+        <v>34</v>
+      </c>
+      <c r="C112" t="n">
+        <v>38</v>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>follow_stag</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="inlineStr">
+        <is>
+          <t>-N600o4FxuE9h8-DIyxx</t>
+        </is>
+      </c>
+      <c r="B113" t="n">
+        <v>12</v>
+      </c>
+      <c r="C113" t="n">
+        <v>22</v>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>random</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="inlineStr">
+        <is>
+          <t>-N600ut0y9Z4gOYIyiuq</t>
+        </is>
+      </c>
+      <c r="B114" t="n">
+        <v>9</v>
+      </c>
+      <c r="C114" t="n">
+        <v>17</v>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>random</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="inlineStr">
+        <is>
+          <t>-N600zTc43eXAZQsIiBf</t>
+        </is>
+      </c>
+      <c r="B115" t="n">
         <v>10</v>
       </c>
-      <c r="D101" t="inlineStr">
-        <is>
-          <t>closest</t>
+      <c r="C115" t="n">
+        <v>24</v>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>random</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="inlineStr">
+        <is>
+          <t>-N6014T7XN-Yci_M6tLn</t>
+        </is>
+      </c>
+      <c r="B116" t="n">
+        <v>3</v>
+      </c>
+      <c r="C116" t="n">
+        <v>17</v>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>random</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="inlineStr">
+        <is>
+          <t>-N601YNdKBzhyui406Tp</t>
+        </is>
+      </c>
+      <c r="B117" t="n">
+        <v>6</v>
+      </c>
+      <c r="C117" t="n">
+        <v>16</v>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>random</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="inlineStr">
+        <is>
+          <t>-N601goESnQqCFcfJ-t3</t>
+        </is>
+      </c>
+      <c r="B118" t="n">
+        <v>9</v>
+      </c>
+      <c r="C118" t="n">
+        <v>22</v>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>random</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="inlineStr">
+        <is>
+          <t>-N601lJmbtSwYem8DsrX</t>
+        </is>
+      </c>
+      <c r="B119" t="n">
+        <v>12</v>
+      </c>
+      <c r="C119" t="n">
+        <v>21</v>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>random</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="1" t="inlineStr">
+        <is>
+          <t>-N602dhEgC76_1JFMR-Q</t>
+        </is>
+      </c>
+      <c r="B120" t="n">
+        <v>6</v>
+      </c>
+      <c r="C120" t="n">
+        <v>18</v>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>follow_stag</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="1" t="inlineStr">
+        <is>
+          <t>-N605MFTS2FjoN5Wl4nd</t>
+        </is>
+      </c>
+      <c r="B121" t="n">
+        <v>5</v>
+      </c>
+      <c r="C121" t="n">
+        <v>13</v>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>random</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="inlineStr">
+        <is>
+          <t>-N608zZT58boWm4nIERF</t>
+        </is>
+      </c>
+      <c r="B122" t="n">
+        <v>32</v>
+      </c>
+      <c r="C122" t="n">
+        <v>36</v>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>follow_stag</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="inlineStr">
+        <is>
+          <t>-N60B-FXwfl_k6O0agPM</t>
+        </is>
+      </c>
+      <c r="B123" t="n">
+        <v>9</v>
+      </c>
+      <c r="C123" t="n">
+        <v>30</v>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>follow_stag</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="inlineStr">
+        <is>
+          <t>-N60DBw3qxKIlxVPL_io</t>
+        </is>
+      </c>
+      <c r="B124" t="n">
+        <v>11</v>
+      </c>
+      <c r="C124" t="n">
+        <v>23</v>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>random</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="1" t="inlineStr">
+        <is>
+          <t>-N60DUPUy4ZVeAjeD1CB</t>
+        </is>
+      </c>
+      <c r="B125" t="n">
+        <v>27</v>
+      </c>
+      <c r="C125" t="n">
+        <v>32</v>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>follow_stag</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="1" t="inlineStr">
+        <is>
+          <t>-N60DjzerUzyJ9ekuEoF</t>
+        </is>
+      </c>
+      <c r="B126" t="n">
+        <v>34</v>
+      </c>
+      <c r="C126" t="n">
+        <v>25</v>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>closest</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="inlineStr">
+        <is>
+          <t>-N60Duj8vhyIzhwaIZQc</t>
+        </is>
+      </c>
+      <c r="B127" t="n">
+        <v>27</v>
+      </c>
+      <c r="C127" t="n">
+        <v>29</v>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>follow_stag</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="1" t="inlineStr">
+        <is>
+          <t>-N60ETyUPyoTeUbk2ErQ</t>
+        </is>
+      </c>
+      <c r="B128" t="n">
+        <v>28</v>
+      </c>
+      <c r="C128" t="n">
+        <v>23</v>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>closest</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="inlineStr">
+        <is>
+          <t>-N60ErvzvYx_bVSDKugG</t>
+        </is>
+      </c>
+      <c r="B129" t="n">
+        <v>9</v>
+      </c>
+      <c r="C129" t="n">
+        <v>29</v>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>follow_stag</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="inlineStr">
+        <is>
+          <t>-N60G23nZZuBppjDOofN</t>
+        </is>
+      </c>
+      <c r="B130" t="n">
+        <v>31</v>
+      </c>
+      <c r="C130" t="n">
+        <v>16</v>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>closest</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="1" t="inlineStr">
+        <is>
+          <t>-N60HPdF56iDJ01ollY0</t>
+        </is>
+      </c>
+      <c r="B131" t="n">
+        <v>7</v>
+      </c>
+      <c r="C131" t="n">
+        <v>25</v>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>follow_stag</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="inlineStr">
+        <is>
+          <t>-N60KUIWwsqc8zGiFzNG</t>
+        </is>
+      </c>
+      <c r="B132" t="n">
+        <v>5</v>
+      </c>
+      <c r="C132" t="n">
+        <v>18</v>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>random</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="1" t="inlineStr">
+        <is>
+          <t>-N60KuKmqPd_41fLQthi</t>
+        </is>
+      </c>
+      <c r="B133" t="n">
+        <v>26</v>
+      </c>
+      <c r="C133" t="n">
+        <v>19</v>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>closest</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="inlineStr">
+        <is>
+          <t>-N60Tx4zmO5_1Fgp6JlT</t>
+        </is>
+      </c>
+      <c r="B134" t="n">
+        <v>27</v>
+      </c>
+      <c r="C134" t="n">
+        <v>31</v>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>closest</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="1" t="inlineStr">
+        <is>
+          <t>-N60UdZtsvjhImC1NplA</t>
+        </is>
+      </c>
+      <c r="B135" t="n">
+        <v>25</v>
+      </c>
+      <c r="C135" t="n">
+        <v>19</v>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>closest</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="1" t="inlineStr">
+        <is>
+          <t>-N611yMxdy44Ur-GYHEH</t>
+        </is>
+      </c>
+      <c r="B136" t="n">
+        <v>5</v>
+      </c>
+      <c r="C136" t="n">
+        <v>17</v>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>random</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="1" t="inlineStr">
+        <is>
+          <t>-N613eK641CjDIG7Sh5G</t>
+        </is>
+      </c>
+      <c r="B137" t="n">
+        <v>4</v>
+      </c>
+      <c r="C137" t="n">
+        <v>21</v>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>random</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Reward of capture the stag is 4 and human model is better and normalized
</commit_message>
<xml_diff>
--- a/python_code/data/all_agents_score.xlsx
+++ b/python_code/data/all_agents_score.xlsx
@@ -457,10 +457,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="C2" t="n">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -475,10 +475,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C3" t="n">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -493,10 +493,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -511,10 +511,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -583,10 +583,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C9" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -619,10 +619,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C11" t="n">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -727,10 +727,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C17" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -745,10 +745,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C18" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -781,10 +781,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C20" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -817,10 +817,10 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C22" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -889,10 +889,10 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C26" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -907,10 +907,10 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C27" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -925,10 +925,10 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C28" t="n">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -943,10 +943,10 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C29" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -1033,10 +1033,10 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C34" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -1069,10 +1069,10 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C36" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -1087,10 +1087,10 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C37" t="n">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -1141,10 +1141,10 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C40" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -1159,10 +1159,10 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C41" t="n">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -1195,10 +1195,10 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C43" t="n">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -1231,10 +1231,10 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C45" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
@@ -1249,10 +1249,10 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C46" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -1267,10 +1267,10 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C47" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -1285,10 +1285,10 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C48" t="n">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
@@ -1303,10 +1303,10 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C49" t="n">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
@@ -1429,10 +1429,10 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C56" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -1447,10 +1447,10 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C57" t="n">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
@@ -1465,10 +1465,10 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C58" t="n">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -1519,10 +1519,10 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C61" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
@@ -1573,10 +1573,10 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C64" t="n">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
@@ -1753,10 +1753,10 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C74" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
@@ -1771,10 +1771,10 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C75" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
@@ -1807,10 +1807,10 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C77" t="n">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
@@ -1843,10 +1843,10 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C79" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
@@ -1861,10 +1861,10 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C80" t="n">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
@@ -1879,10 +1879,10 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C81" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
@@ -1897,10 +1897,10 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C82" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
@@ -1969,10 +1969,10 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C86" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
@@ -1987,10 +1987,10 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C87" t="n">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
@@ -2005,10 +2005,10 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="C88" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
@@ -2023,10 +2023,10 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C89" t="n">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
@@ -2041,10 +2041,10 @@
         </is>
       </c>
       <c r="B90" t="n">
+        <v>31</v>
+      </c>
+      <c r="C90" t="n">
         <v>30</v>
-      </c>
-      <c r="C90" t="n">
-        <v>29</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
@@ -2059,10 +2059,10 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C91" t="n">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
@@ -2077,10 +2077,10 @@
         </is>
       </c>
       <c r="B92" t="n">
+        <v>39</v>
+      </c>
+      <c r="C92" t="n">
         <v>36</v>
-      </c>
-      <c r="C92" t="n">
-        <v>33</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
@@ -2167,10 +2167,10 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C97" t="n">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
@@ -2185,10 +2185,10 @@
         </is>
       </c>
       <c r="B98" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C98" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D98" t="inlineStr">
         <is>
@@ -2203,10 +2203,10 @@
         </is>
       </c>
       <c r="B99" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C99" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D99" t="inlineStr">
         <is>
@@ -2257,10 +2257,10 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C102" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D102" t="inlineStr">
         <is>
@@ -2275,10 +2275,10 @@
         </is>
       </c>
       <c r="B103" t="n">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C103" t="n">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="D103" t="inlineStr">
         <is>
@@ -2329,10 +2329,10 @@
         </is>
       </c>
       <c r="B106" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C106" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D106" t="inlineStr">
         <is>
@@ -2347,10 +2347,10 @@
         </is>
       </c>
       <c r="B107" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C107" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D107" t="inlineStr">
         <is>
@@ -2401,10 +2401,10 @@
         </is>
       </c>
       <c r="B110" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C110" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D110" t="inlineStr">
         <is>
@@ -2419,10 +2419,10 @@
         </is>
       </c>
       <c r="B111" t="n">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C111" t="n">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="D111" t="inlineStr">
         <is>
@@ -2437,10 +2437,10 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="C112" t="n">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="D112" t="inlineStr">
         <is>
@@ -2455,10 +2455,10 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C113" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D113" t="inlineStr">
         <is>
@@ -2473,10 +2473,10 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C114" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D114" t="inlineStr">
         <is>
@@ -2491,10 +2491,10 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C115" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D115" t="inlineStr">
         <is>
@@ -2545,10 +2545,10 @@
         </is>
       </c>
       <c r="B118" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C118" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D118" t="inlineStr">
         <is>
@@ -2563,10 +2563,10 @@
         </is>
       </c>
       <c r="B119" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C119" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D119" t="inlineStr">
         <is>
@@ -2617,10 +2617,10 @@
         </is>
       </c>
       <c r="B122" t="n">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C122" t="n">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="D122" t="inlineStr">
         <is>
@@ -2635,10 +2635,10 @@
         </is>
       </c>
       <c r="B123" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C123" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D123" t="inlineStr">
         <is>
@@ -2653,10 +2653,10 @@
         </is>
       </c>
       <c r="B124" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C124" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D124" t="inlineStr">
         <is>
@@ -2671,10 +2671,10 @@
         </is>
       </c>
       <c r="B125" t="n">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="C125" t="n">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="D125" t="inlineStr">
         <is>
@@ -2707,10 +2707,10 @@
         </is>
       </c>
       <c r="B127" t="n">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="C127" t="n">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="D127" t="inlineStr">
         <is>
@@ -2743,10 +2743,10 @@
         </is>
       </c>
       <c r="B129" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C129" t="n">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D129" t="inlineStr">
         <is>
@@ -2779,10 +2779,10 @@
         </is>
       </c>
       <c r="B131" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C131" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D131" t="inlineStr">
         <is>
@@ -2815,10 +2815,10 @@
         </is>
       </c>
       <c r="B133" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C133" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D133" t="inlineStr">
         <is>
@@ -2833,10 +2833,10 @@
         </is>
       </c>
       <c r="B134" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C134" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D134" t="inlineStr">
         <is>
@@ -2851,10 +2851,10 @@
         </is>
       </c>
       <c r="B135" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C135" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D135" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
change in js to reward of cupture flag to 5 and update firebase with fix scores
</commit_message>
<xml_diff>
--- a/python_code/data/all_agents_score.xlsx
+++ b/python_code/data/all_agents_score.xlsx
@@ -457,10 +457,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="C2" t="n">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -475,10 +475,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C3" t="n">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -493,10 +493,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -511,10 +511,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -583,10 +583,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C9" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -619,10 +619,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C11" t="n">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -727,10 +727,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C17" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -745,10 +745,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C18" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -781,10 +781,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C20" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -817,10 +817,10 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C22" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -889,10 +889,10 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C26" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -907,10 +907,10 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C27" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -925,10 +925,10 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C28" t="n">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -943,10 +943,10 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C29" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -1033,10 +1033,10 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C34" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -1069,10 +1069,10 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C36" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -1087,10 +1087,10 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C37" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -1141,10 +1141,10 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C40" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -1159,10 +1159,10 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C41" t="n">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -1195,10 +1195,10 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C43" t="n">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -1231,10 +1231,10 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C45" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
@@ -1249,10 +1249,10 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C46" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -1267,10 +1267,10 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C47" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -1285,10 +1285,10 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C48" t="n">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
@@ -1303,10 +1303,10 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C49" t="n">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
@@ -1429,10 +1429,10 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C56" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -1447,10 +1447,10 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C57" t="n">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
@@ -1465,10 +1465,10 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C58" t="n">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -1519,10 +1519,10 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C61" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
@@ -1573,10 +1573,10 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C64" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
@@ -1753,10 +1753,10 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C74" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
@@ -1771,10 +1771,10 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C75" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
@@ -1807,10 +1807,10 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C77" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
@@ -1843,10 +1843,10 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C79" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
@@ -1861,10 +1861,10 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="C80" t="n">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
@@ -1879,10 +1879,10 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C81" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
@@ -1897,10 +1897,10 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C82" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
@@ -1969,10 +1969,10 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C86" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
@@ -1987,10 +1987,10 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C87" t="n">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
@@ -2005,10 +2005,10 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="C88" t="n">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
@@ -2023,10 +2023,10 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C89" t="n">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
@@ -2041,10 +2041,10 @@
         </is>
       </c>
       <c r="B90" t="n">
+        <v>32</v>
+      </c>
+      <c r="C90" t="n">
         <v>31</v>
-      </c>
-      <c r="C90" t="n">
-        <v>30</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
@@ -2059,10 +2059,10 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C91" t="n">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
@@ -2077,10 +2077,10 @@
         </is>
       </c>
       <c r="B92" t="n">
+        <v>42</v>
+      </c>
+      <c r="C92" t="n">
         <v>39</v>
-      </c>
-      <c r="C92" t="n">
-        <v>36</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
@@ -2167,10 +2167,10 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C97" t="n">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
@@ -2185,10 +2185,10 @@
         </is>
       </c>
       <c r="B98" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C98" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D98" t="inlineStr">
         <is>
@@ -2203,10 +2203,10 @@
         </is>
       </c>
       <c r="B99" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C99" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D99" t="inlineStr">
         <is>
@@ -2257,10 +2257,10 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C102" t="n">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D102" t="inlineStr">
         <is>
@@ -2275,10 +2275,10 @@
         </is>
       </c>
       <c r="B103" t="n">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="C103" t="n">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="D103" t="inlineStr">
         <is>
@@ -2329,10 +2329,10 @@
         </is>
       </c>
       <c r="B106" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C106" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D106" t="inlineStr">
         <is>
@@ -2347,10 +2347,10 @@
         </is>
       </c>
       <c r="B107" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C107" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D107" t="inlineStr">
         <is>
@@ -2401,10 +2401,10 @@
         </is>
       </c>
       <c r="B110" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C110" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D110" t="inlineStr">
         <is>
@@ -2419,10 +2419,10 @@
         </is>
       </c>
       <c r="B111" t="n">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="C111" t="n">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="D111" t="inlineStr">
         <is>
@@ -2437,10 +2437,10 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="C112" t="n">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="D112" t="inlineStr">
         <is>
@@ -2455,10 +2455,10 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C113" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D113" t="inlineStr">
         <is>
@@ -2473,10 +2473,10 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C114" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D114" t="inlineStr">
         <is>
@@ -2491,10 +2491,10 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C115" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D115" t="inlineStr">
         <is>
@@ -2545,10 +2545,10 @@
         </is>
       </c>
       <c r="B118" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C118" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D118" t="inlineStr">
         <is>
@@ -2563,10 +2563,10 @@
         </is>
       </c>
       <c r="B119" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C119" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D119" t="inlineStr">
         <is>
@@ -2617,10 +2617,10 @@
         </is>
       </c>
       <c r="B122" t="n">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C122" t="n">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="D122" t="inlineStr">
         <is>
@@ -2635,10 +2635,10 @@
         </is>
       </c>
       <c r="B123" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C123" t="n">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D123" t="inlineStr">
         <is>
@@ -2653,10 +2653,10 @@
         </is>
       </c>
       <c r="B124" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C124" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D124" t="inlineStr">
         <is>
@@ -2671,10 +2671,10 @@
         </is>
       </c>
       <c r="B125" t="n">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="C125" t="n">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="D125" t="inlineStr">
         <is>
@@ -2707,10 +2707,10 @@
         </is>
       </c>
       <c r="B127" t="n">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C127" t="n">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="D127" t="inlineStr">
         <is>
@@ -2743,10 +2743,10 @@
         </is>
       </c>
       <c r="B129" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C129" t="n">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D129" t="inlineStr">
         <is>
@@ -2779,10 +2779,10 @@
         </is>
       </c>
       <c r="B131" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C131" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D131" t="inlineStr">
         <is>
@@ -2815,10 +2815,10 @@
         </is>
       </c>
       <c r="B133" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C133" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D133" t="inlineStr">
         <is>
@@ -2833,10 +2833,10 @@
         </is>
       </c>
       <c r="B134" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C134" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D134" t="inlineStr">
         <is>
@@ -2851,10 +2851,10 @@
         </is>
       </c>
       <c r="B135" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C135" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D135" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
train human model v2
</commit_message>
<xml_diff>
--- a/python_code/data/all_agents_score.xlsx
+++ b/python_code/data/all_agents_score.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D137"/>
+  <dimension ref="A1:D153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2883,18 +2883,306 @@
     <row r="137">
       <c r="A137" s="1" t="inlineStr">
         <is>
-          <t>-N613eK641CjDIG7Sh5G</t>
+          <t>-N7S6teeioJOgwOkGHeb</t>
         </is>
       </c>
       <c r="B137" t="n">
+        <v>54</v>
+      </c>
+      <c r="C137" t="n">
+        <v>59</v>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>follow_stag</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="1" t="inlineStr">
+        <is>
+          <t>-N7S6zxhC8D9WPKQ1GTJ</t>
+        </is>
+      </c>
+      <c r="B138" t="n">
+        <v>25</v>
+      </c>
+      <c r="C138" t="n">
+        <v>24</v>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>closest</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="1" t="inlineStr">
+        <is>
+          <t>-N7S7QCaT2R-cN-xQoen</t>
+        </is>
+      </c>
+      <c r="B139" t="n">
+        <v>5</v>
+      </c>
+      <c r="C139" t="n">
+        <v>8</v>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>random</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="1" t="inlineStr">
+        <is>
+          <t>-N7S8YwrV6R9W4BW1dzL</t>
+        </is>
+      </c>
+      <c r="B140" t="n">
+        <v>9</v>
+      </c>
+      <c r="C140" t="n">
+        <v>25</v>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>follow_stag</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="1" t="inlineStr">
+        <is>
+          <t>-N7S92Id30UECmsUw1ZJ</t>
+        </is>
+      </c>
+      <c r="B141" t="n">
+        <v>62</v>
+      </c>
+      <c r="C141" t="n">
+        <v>61</v>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>follow_stag</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="1" t="inlineStr">
+        <is>
+          <t>-N7SAbmiI0l11nqFTIxY</t>
+        </is>
+      </c>
+      <c r="B142" t="n">
+        <v>6</v>
+      </c>
+      <c r="C142" t="n">
+        <v>31</v>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>follow_stag</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="1" t="inlineStr">
+        <is>
+          <t>-N7SDLpwrkF3J6tlEbbg</t>
+        </is>
+      </c>
+      <c r="B143" t="n">
+        <v>42</v>
+      </c>
+      <c r="C143" t="n">
+        <v>48</v>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>follow_stag</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="1" t="inlineStr">
+        <is>
+          <t>-N7SE7P1i5pBPagbU2fs</t>
+        </is>
+      </c>
+      <c r="B144" t="n">
+        <v>7</v>
+      </c>
+      <c r="C144" t="n">
+        <v>22</v>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>random</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="1" t="inlineStr">
+        <is>
+          <t>-N7SG-gcyIrxsm71UJ70</t>
+        </is>
+      </c>
+      <c r="B145" t="n">
         <v>4</v>
       </c>
-      <c r="C137" t="n">
-        <v>21</v>
-      </c>
-      <c r="D137" t="inlineStr">
-        <is>
-          <t>random</t>
+      <c r="C145" t="n">
+        <v>19</v>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>follow_stag</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="1" t="inlineStr">
+        <is>
+          <t>-N7SKdAU00pOm8Cdx2lf</t>
+        </is>
+      </c>
+      <c r="B146" t="n">
+        <v>5</v>
+      </c>
+      <c r="C146" t="n">
+        <v>22</v>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>random</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="1" t="inlineStr">
+        <is>
+          <t>-N7SNi9HqPWM2I4geMxR</t>
+        </is>
+      </c>
+      <c r="B147" t="n">
+        <v>8</v>
+      </c>
+      <c r="C147" t="n">
+        <v>24</v>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>random</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="1" t="inlineStr">
+        <is>
+          <t>-N7SQQHk7nWiuDwke8jf</t>
+        </is>
+      </c>
+      <c r="B148" t="n">
+        <v>25</v>
+      </c>
+      <c r="C148" t="n">
+        <v>19</v>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>closest</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="1" t="inlineStr">
+        <is>
+          <t>-N7SS0ZNRRzABEFqOvRm</t>
+        </is>
+      </c>
+      <c r="B149" t="n">
+        <v>37</v>
+      </c>
+      <c r="C149" t="n">
+        <v>51</v>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>follow_stag</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="1" t="inlineStr">
+        <is>
+          <t>-N7SWDA_ldwYcJkG2XKL</t>
+        </is>
+      </c>
+      <c r="B150" t="n">
+        <v>57</v>
+      </c>
+      <c r="C150" t="n">
+        <v>57</v>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>follow_stag</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="1" t="inlineStr">
+        <is>
+          <t>-N7SZPE3oHGDDzPTrYxV</t>
+        </is>
+      </c>
+      <c r="B151" t="n">
+        <v>7</v>
+      </c>
+      <c r="C151" t="n">
+        <v>19</v>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>random</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="1" t="inlineStr">
+        <is>
+          <t>-N7ScVpejC0Dy0ua8k1T</t>
+        </is>
+      </c>
+      <c r="B152" t="n">
+        <v>56</v>
+      </c>
+      <c r="C152" t="n">
+        <v>55</v>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>follow_stag</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="1" t="inlineStr">
+        <is>
+          <t>-N7SuS0uDb2PVST69Iae</t>
+        </is>
+      </c>
+      <c r="B153" t="n">
+        <v>5</v>
+      </c>
+      <c r="C153" t="n">
+        <v>25</v>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>follow_stag</t>
         </is>
       </c>
     </row>

</xml_diff>